<commit_message>
Updates to formatted tables
Added word doc to repo and updated tables in MS Word version
</commit_message>
<xml_diff>
--- a/docs/TL_modeling_summary_table.xlsx
+++ b/docs/TL_modeling_summary_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
   <si>
     <t>Network</t>
   </si>
@@ -159,8 +159,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="mm/yyyy"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -279,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -330,70 +330,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -403,34 +373,91 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -714,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N12"/>
+  <dimension ref="B1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,7 +758,7 @@
     <col min="9" max="9" width="10.77734375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="2" customFormat="1" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:14" s="2" customFormat="1" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,36 +783,26 @@
       <c r="I1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
     </row>
     <row r="2" spans="2:14" s="3" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="24">
         <v>43299</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="43">
         <v>1.22</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="48">
         <v>19.5</v>
       </c>
       <c r="G2" s="5">
@@ -797,63 +814,43 @@
       <c r="I2" s="14">
         <v>1.63</v>
       </c>
-      <c r="J2" s="10">
-        <v>208</v>
-      </c>
-      <c r="K2" s="10">
-        <v>41</v>
-      </c>
-      <c r="L2" s="10">
-        <v>14</v>
-      </c>
-      <c r="M2" s="36">
-        <v>0.197115384615384</v>
-      </c>
-      <c r="N2" s="36">
-        <v>0.36585365853658502</v>
-      </c>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
     </row>
     <row r="3" spans="2:14" s="3" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="33">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="23">
         <v>43435</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="24"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="49"/>
       <c r="G3" s="12">
         <v>250</v>
       </c>
       <c r="H3" s="12">
         <v>84.1</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="22">
         <v>1.89</v>
       </c>
-      <c r="J3" s="10">
-        <v>216</v>
-      </c>
-      <c r="K3" s="10">
-        <v>33</v>
-      </c>
-      <c r="L3" s="10">
-        <v>0</v>
-      </c>
-      <c r="M3" s="36">
-        <v>0.15277777777777701</v>
-      </c>
-      <c r="N3" s="36">
-        <v>0.66666666666666596</v>
-      </c>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
     </row>
     <row r="4" spans="2:14" s="3" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="28"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="33">
+      <c r="B4" s="42"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="23">
         <v>43556</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="25"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="50"/>
       <c r="G4" s="12">
         <v>250</v>
       </c>
@@ -863,34 +860,24 @@
       <c r="I4" s="10">
         <v>1.73</v>
       </c>
-      <c r="J4" s="10">
-        <v>326</v>
-      </c>
-      <c r="K4" s="10">
-        <v>57</v>
-      </c>
-      <c r="L4" s="10">
-        <v>31</v>
-      </c>
-      <c r="M4" s="36">
-        <v>0.17484662576687099</v>
-      </c>
-      <c r="N4" s="36">
-        <v>0.57894736842105199</v>
-      </c>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
     </row>
     <row r="5" spans="2:14" s="3" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="28"/>
-      <c r="C5" s="28" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="23">
         <v>43313</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="46">
         <v>0.76</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="51">
         <v>17.7</v>
       </c>
       <c r="G5" s="12">
@@ -902,30 +889,20 @@
       <c r="I5" s="10">
         <v>1.39</v>
       </c>
-      <c r="J5" s="10">
-        <v>112</v>
-      </c>
-      <c r="K5" s="10">
-        <v>41</v>
-      </c>
-      <c r="L5" s="10">
-        <v>8</v>
-      </c>
-      <c r="M5" s="36">
-        <v>0.36607142857142799</v>
-      </c>
-      <c r="N5" s="36">
-        <v>0.292682926829268</v>
-      </c>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
     </row>
     <row r="6" spans="2:14" s="3" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="33">
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="23">
         <v>43435</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="24"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="49"/>
       <c r="G6" s="12">
         <v>200</v>
       </c>
@@ -935,30 +912,20 @@
       <c r="I6" s="10">
         <v>1.84</v>
       </c>
-      <c r="J6" s="10">
-        <v>265</v>
-      </c>
-      <c r="K6" s="10">
-        <v>42</v>
-      </c>
-      <c r="L6" s="10">
-        <v>29</v>
-      </c>
-      <c r="M6" s="36">
-        <v>0.15849056603773501</v>
-      </c>
-      <c r="N6" s="36">
-        <v>0.71428571428571397</v>
-      </c>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
     </row>
     <row r="7" spans="2:14" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="35">
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="25">
         <v>43617</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="27"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="13">
         <v>200</v>
       </c>
@@ -968,30 +935,20 @@
       <c r="I7" s="11">
         <v>1.32</v>
       </c>
-      <c r="J7" s="11">
-        <v>241</v>
-      </c>
-      <c r="K7" s="11">
-        <v>75</v>
-      </c>
-      <c r="L7" s="11">
-        <v>65</v>
-      </c>
-      <c r="M7" s="37">
-        <v>0.31120331950207403</v>
-      </c>
-      <c r="N7" s="37">
-        <v>0.90666666666666595</v>
-      </c>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
     </row>
     <row r="8" spans="2:14" s="3" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="40" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="24">
         <v>44075</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -1009,28 +966,18 @@
       <c r="I8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="14">
-        <v>125</v>
-      </c>
-      <c r="K8" s="14">
-        <v>7</v>
-      </c>
-      <c r="L8" s="14">
-        <v>3</v>
-      </c>
-      <c r="M8" s="38">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="N8" s="38">
-        <v>0.42859999999999998</v>
-      </c>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
     </row>
     <row r="9" spans="2:14" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="29"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="25">
         <v>43709</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -1048,30 +995,20 @@
       <c r="I9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="11">
-        <v>109</v>
-      </c>
-      <c r="K9" s="11">
-        <v>4</v>
-      </c>
-      <c r="L9" s="11">
-        <v>2</v>
-      </c>
-      <c r="M9" s="37">
-        <v>3.6700000000000003E-2</v>
-      </c>
-      <c r="N9" s="37">
-        <v>0.5</v>
-      </c>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="59"/>
     </row>
     <row r="10" spans="2:14" s="3" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="24">
         <v>44562</v>
       </c>
       <c r="E10" s="14">
@@ -1089,28 +1026,18 @@
       <c r="I10" s="16">
         <v>39.5</v>
       </c>
-      <c r="J10" s="16">
-        <v>390</v>
-      </c>
-      <c r="K10" s="16">
-        <v>1</v>
-      </c>
-      <c r="L10" s="16">
-        <v>0</v>
-      </c>
-      <c r="M10" s="39">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="N10" s="39">
-        <v>0</v>
-      </c>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14" s="3" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="28"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="23">
         <v>44562</v>
       </c>
       <c r="E11" s="10" t="s">
@@ -1128,28 +1055,18 @@
       <c r="I11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="10">
-        <v>345</v>
-      </c>
-      <c r="K11" s="10">
-        <v>21</v>
-      </c>
-      <c r="L11" s="10">
-        <v>3</v>
-      </c>
-      <c r="M11" s="36">
-        <v>6.0900000000000003E-2</v>
-      </c>
-      <c r="N11" s="36">
-        <v>0.1429</v>
-      </c>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
     </row>
     <row r="12" spans="2:14" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="29"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="25">
         <v>44317</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -1167,24 +1084,307 @@
       <c r="I12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="59"/>
+    </row>
+    <row r="22" spans="2:9" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="24">
+        <v>43299</v>
+      </c>
+      <c r="E23" s="18">
+        <v>208</v>
+      </c>
+      <c r="F23" s="18">
+        <v>41</v>
+      </c>
+      <c r="G23" s="18">
+        <v>14</v>
+      </c>
+      <c r="H23" s="26">
+        <v>0.197115384615384</v>
+      </c>
+      <c r="I23" s="26">
+        <v>0.36585365853658502</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="23">
+        <v>43435</v>
+      </c>
+      <c r="E24" s="18">
+        <v>216</v>
+      </c>
+      <c r="F24" s="18">
+        <v>33</v>
+      </c>
+      <c r="G24" s="18">
+        <v>0</v>
+      </c>
+      <c r="H24" s="26">
+        <v>0.15277777777777701</v>
+      </c>
+      <c r="I24" s="26">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="42"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="23">
+        <v>43556</v>
+      </c>
+      <c r="E25" s="18">
+        <v>326</v>
+      </c>
+      <c r="F25" s="18">
+        <v>57</v>
+      </c>
+      <c r="G25" s="18">
+        <v>31</v>
+      </c>
+      <c r="H25" s="26">
+        <v>0.17484662576687099</v>
+      </c>
+      <c r="I25" s="26">
+        <v>0.57894736842105199</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="42"/>
+      <c r="C26" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="23">
+        <v>43313</v>
+      </c>
+      <c r="E26" s="18">
+        <v>112</v>
+      </c>
+      <c r="F26" s="18">
+        <v>41</v>
+      </c>
+      <c r="G26" s="18">
+        <v>8</v>
+      </c>
+      <c r="H26" s="26">
+        <v>0.36607142857142799</v>
+      </c>
+      <c r="I26" s="26">
+        <v>0.292682926829268</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="23">
+        <v>43435</v>
+      </c>
+      <c r="E27" s="18">
+        <v>265</v>
+      </c>
+      <c r="F27" s="18">
+        <v>42</v>
+      </c>
+      <c r="G27" s="18">
+        <v>29</v>
+      </c>
+      <c r="H27" s="26">
+        <v>0.15849056603773501</v>
+      </c>
+      <c r="I27" s="26">
+        <v>0.71428571428571397</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="25">
+        <v>43617</v>
+      </c>
+      <c r="E28" s="19">
+        <v>241</v>
+      </c>
+      <c r="F28" s="19">
+        <v>75</v>
+      </c>
+      <c r="G28" s="19">
+        <v>65</v>
+      </c>
+      <c r="H28" s="27">
+        <v>0.31120331950207403</v>
+      </c>
+      <c r="I28" s="27">
+        <v>0.90666666666666595</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="24">
+        <v>44075</v>
+      </c>
+      <c r="E29" s="14">
+        <v>125</v>
+      </c>
+      <c r="F29" s="14">
+        <v>7</v>
+      </c>
+      <c r="G29" s="14">
+        <v>3</v>
+      </c>
+      <c r="H29" s="28">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I29" s="28">
+        <v>0.42859999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="41"/>
+      <c r="C30" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="25">
+        <v>43709</v>
+      </c>
+      <c r="E30" s="19">
+        <v>109</v>
+      </c>
+      <c r="F30" s="19">
+        <v>4</v>
+      </c>
+      <c r="G30" s="19">
+        <v>2</v>
+      </c>
+      <c r="H30" s="27">
+        <v>3.6700000000000003E-2</v>
+      </c>
+      <c r="I30" s="27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B31" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="24">
+        <v>44562</v>
+      </c>
+      <c r="E31" s="16">
+        <v>390</v>
+      </c>
+      <c r="F31" s="16">
+        <v>1</v>
+      </c>
+      <c r="G31" s="16">
+        <v>0</v>
+      </c>
+      <c r="H31" s="29">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="I31" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B32" s="42"/>
+      <c r="C32" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="23">
+        <v>44562</v>
+      </c>
+      <c r="E32" s="18">
+        <v>345</v>
+      </c>
+      <c r="F32" s="18">
+        <v>21</v>
+      </c>
+      <c r="G32" s="18">
+        <v>3</v>
+      </c>
+      <c r="H32" s="26">
+        <v>6.0900000000000003E-2</v>
+      </c>
+      <c r="I32" s="26">
+        <v>0.1429</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="41"/>
+      <c r="C33" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="25">
+        <v>44317</v>
+      </c>
+      <c r="E33" s="19">
         <v>831</v>
       </c>
-      <c r="K12" s="11">
+      <c r="F33" s="19">
         <v>61</v>
       </c>
-      <c r="L12" s="11">
+      <c r="G33" s="19">
         <v>52</v>
       </c>
-      <c r="M12" s="37">
+      <c r="H33" s="27">
         <v>7.3400000000000007E-2</v>
       </c>
-      <c r="N12" s="37">
+      <c r="I33" s="27">
         <v>0.85250000000000004</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="14">
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B33"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="E2:E4"/>
@@ -1205,467 +1405,467 @@
   <dimension ref="B2:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="40"/>
-    <col min="2" max="2" width="20.21875" style="40" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="40"/>
+    <col min="1" max="1" width="8.88671875" style="30"/>
+    <col min="2" max="2" width="20.21875" style="30" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="30"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42" t="s">
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42" t="s">
+      <c r="J2" s="55"/>
+      <c r="K2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42" t="s">
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="43" t="s">
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="33">
         <v>43299</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="33">
         <v>43435</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="33">
         <v>43556</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="33">
         <v>43313</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="33">
         <v>43435</v>
       </c>
-      <c r="H4" s="44">
+      <c r="H4" s="33">
         <v>43617</v>
       </c>
-      <c r="I4" s="44">
+      <c r="I4" s="33">
         <v>44075</v>
       </c>
-      <c r="J4" s="44">
+      <c r="J4" s="33">
         <v>43709</v>
       </c>
-      <c r="K4" s="44">
+      <c r="K4" s="33">
         <v>44562</v>
       </c>
-      <c r="L4" s="44">
+      <c r="L4" s="33">
         <v>44562</v>
       </c>
-      <c r="M4" s="44">
+      <c r="M4" s="33">
         <v>44317</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="56">
         <v>1.22</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46">
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56">
         <v>0.76</v>
       </c>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47" t="s">
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="48" t="s">
+      <c r="J5" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="48">
+      <c r="K5" s="36">
         <v>2.13</v>
       </c>
-      <c r="L5" s="48" t="s">
+      <c r="L5" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="48" t="s">
+      <c r="M5" s="36" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="54">
         <v>19.5</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49">
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54">
         <v>17.7</v>
       </c>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="47">
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="35">
         <v>17.399999999999999</v>
       </c>
-      <c r="J6" s="47">
+      <c r="J6" s="35">
         <v>16.399999999999999</v>
       </c>
-      <c r="K6" s="47">
+      <c r="K6" s="35">
         <v>10.9</v>
       </c>
-      <c r="L6" s="47">
+      <c r="L6" s="35">
         <v>14.95</v>
       </c>
-      <c r="M6" s="47" t="s">
+      <c r="M6" s="35" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="35">
         <v>250</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="35">
         <v>250</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="35">
         <v>250</v>
       </c>
-      <c r="F7" s="47">
+      <c r="F7" s="35">
         <v>200</v>
       </c>
-      <c r="G7" s="47">
+      <c r="G7" s="35">
         <v>200</v>
       </c>
-      <c r="H7" s="47">
+      <c r="H7" s="35">
         <v>200</v>
       </c>
-      <c r="I7" s="47">
+      <c r="I7" s="35">
         <v>200</v>
       </c>
-      <c r="J7" s="47">
+      <c r="J7" s="35">
         <v>500</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="35">
         <v>160</v>
       </c>
-      <c r="L7" s="47">
+      <c r="L7" s="35">
         <v>100</v>
       </c>
-      <c r="M7" s="47">
+      <c r="M7" s="35">
         <v>250</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="35">
         <v>87.7</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="35">
         <v>84.1</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="35">
         <v>86.4</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="35">
         <v>91.3</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="35">
         <v>83.4</v>
       </c>
-      <c r="H8" s="47">
+      <c r="H8" s="35">
         <v>92.7</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="35">
         <v>75.599999999999994</v>
       </c>
-      <c r="L8" s="47" t="s">
+      <c r="L8" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="M8" s="47" t="s">
+      <c r="M8" s="35" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="48">
+      <c r="C9" s="36">
         <v>1.63</v>
       </c>
-      <c r="D9" s="50">
+      <c r="D9" s="37">
         <v>1.89</v>
       </c>
-      <c r="E9" s="48">
+      <c r="E9" s="36">
         <v>1.73</v>
       </c>
-      <c r="F9" s="48">
+      <c r="F9" s="36">
         <v>1.39</v>
       </c>
-      <c r="G9" s="48">
+      <c r="G9" s="36">
         <v>1.84</v>
       </c>
-      <c r="H9" s="48">
+      <c r="H9" s="36">
         <v>1.32</v>
       </c>
-      <c r="I9" s="48" t="s">
+      <c r="I9" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="48" t="s">
+      <c r="J9" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="50">
+      <c r="K9" s="37">
         <v>39.5</v>
       </c>
-      <c r="L9" s="48" t="s">
+      <c r="L9" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="48" t="s">
+      <c r="M9" s="36" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="48">
+      <c r="C10" s="36">
         <v>208</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="36">
         <v>216</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="36">
         <v>326</v>
       </c>
-      <c r="F10" s="48">
+      <c r="F10" s="36">
         <v>112</v>
       </c>
-      <c r="G10" s="48">
+      <c r="G10" s="36">
         <v>265</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10" s="36">
         <v>241</v>
       </c>
-      <c r="I10" s="48">
+      <c r="I10" s="36">
         <v>125</v>
       </c>
-      <c r="J10" s="48">
+      <c r="J10" s="36">
         <v>109</v>
       </c>
-      <c r="K10" s="50">
+      <c r="K10" s="37">
         <v>390</v>
       </c>
-      <c r="L10" s="48">
+      <c r="L10" s="36">
         <v>345</v>
       </c>
-      <c r="M10" s="48">
+      <c r="M10" s="36">
         <v>831</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="48">
+      <c r="C11" s="36">
         <v>41</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="36">
         <v>33</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="36">
         <v>57</v>
       </c>
-      <c r="F11" s="48">
+      <c r="F11" s="36">
         <v>41</v>
       </c>
-      <c r="G11" s="48">
+      <c r="G11" s="36">
         <v>42</v>
       </c>
-      <c r="H11" s="48">
+      <c r="H11" s="36">
         <v>75</v>
       </c>
-      <c r="I11" s="48">
+      <c r="I11" s="36">
         <v>7</v>
       </c>
-      <c r="J11" s="48">
+      <c r="J11" s="36">
         <v>4</v>
       </c>
-      <c r="K11" s="50">
+      <c r="K11" s="37">
         <v>1</v>
       </c>
-      <c r="L11" s="48">
+      <c r="L11" s="36">
         <v>21</v>
       </c>
-      <c r="M11" s="48">
+      <c r="M11" s="36">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="48">
+      <c r="C12" s="36">
         <v>14</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="36">
         <v>0</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="36">
         <v>31</v>
       </c>
-      <c r="F12" s="48">
+      <c r="F12" s="36">
         <v>8</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="36">
         <v>29</v>
       </c>
-      <c r="H12" s="48">
+      <c r="H12" s="36">
         <v>65</v>
       </c>
-      <c r="I12" s="48">
+      <c r="I12" s="36">
         <v>3</v>
       </c>
-      <c r="J12" s="48">
+      <c r="J12" s="36">
         <v>2</v>
       </c>
-      <c r="K12" s="50">
+      <c r="K12" s="37">
         <v>0</v>
       </c>
-      <c r="L12" s="48">
+      <c r="L12" s="36">
         <v>3</v>
       </c>
-      <c r="M12" s="48">
+      <c r="M12" s="36">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="38">
         <v>0.197115384615384</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="38">
         <v>0.15277777777777701</v>
       </c>
-      <c r="E13" s="51">
+      <c r="E13" s="38">
         <v>0.17484662576687099</v>
       </c>
-      <c r="F13" s="51">
+      <c r="F13" s="38">
         <v>0.36607142857142799</v>
       </c>
-      <c r="G13" s="51">
+      <c r="G13" s="38">
         <v>0.15849056603773501</v>
       </c>
-      <c r="H13" s="51">
+      <c r="H13" s="38">
         <v>0.31120331950207403</v>
       </c>
-      <c r="I13" s="51">
+      <c r="I13" s="38">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="J13" s="51">
+      <c r="J13" s="38">
         <v>3.6700000000000003E-2</v>
       </c>
-      <c r="K13" s="52">
+      <c r="K13" s="39">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="L13" s="51">
+      <c r="L13" s="38">
         <v>6.0900000000000003E-2</v>
       </c>
-      <c r="M13" s="51">
+      <c r="M13" s="38">
         <v>7.3400000000000007E-2</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14" s="38">
         <v>0.36585365853658502</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="38">
         <v>0.66666666666666596</v>
       </c>
-      <c r="E14" s="51">
+      <c r="E14" s="38">
         <v>0.57894736842105199</v>
       </c>
-      <c r="F14" s="51">
+      <c r="F14" s="38">
         <v>0.292682926829268</v>
       </c>
-      <c r="G14" s="51">
+      <c r="G14" s="38">
         <v>0.71428571428571397</v>
       </c>
-      <c r="H14" s="51">
+      <c r="H14" s="38">
         <v>0.90666666666666595</v>
       </c>
-      <c r="I14" s="51">
+      <c r="I14" s="38">
         <v>0.42859999999999998</v>
       </c>
-      <c r="J14" s="51">
+      <c r="J14" s="38">
         <v>0.5</v>
       </c>
-      <c r="K14" s="52">
+      <c r="K14" s="39">
         <v>0</v>
       </c>
-      <c r="L14" s="51">
+      <c r="L14" s="38">
         <v>0.1429</v>
       </c>
-      <c r="M14" s="51">
+      <c r="M14" s="38">
         <v>0.85250000000000004</v>
       </c>
     </row>

</xml_diff>